<commit_message>
- Possibility to define multiple excel-files (Annotation @ExcelFile is now available for String, List<String> and String[]) - pom.xml: warnings fixed
</commit_message>
<xml_diff>
--- a/src/test/resources/MassTests.xlsx
+++ b/src/test/resources/MassTests.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="10">
   <si>
     <t>Testcase for testing the formula evaluation</t>
   </si>
@@ -39,6 +39,12 @@
   </si>
   <si>
     <t>ADD</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>exception</t>
   </si>
 </sst>
 </file>
@@ -391,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -402,12 +408,12 @@
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -415,7 +421,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -428,8 +434,11 @@
       <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -442,8 +451,11 @@
       <c r="D6">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -457,7 +469,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -472,7 +484,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -487,7 +499,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -502,7 +514,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -517,7 +529,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -532,7 +544,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -547,7 +559,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -562,7 +574,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>

</xml_diff>